<commit_message>
Added counting to Excell sheet
Added the amount of parkingspots to the excellsheet kalkuleringark
</commit_message>
<xml_diff>
--- a/Resurser/kalkuleringsark.xlsx
+++ b/Resurser/kalkuleringsark.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Inspiria</t>
   </si>
@@ -81,6 +82,30 @@
   </si>
   <si>
     <t>Antall</t>
+  </si>
+  <si>
+    <t>Antall Plasser</t>
+  </si>
+  <si>
+    <t>Inspiria Bak</t>
+  </si>
+  <si>
+    <t>Superland</t>
+  </si>
+  <si>
+    <t>K5 Bygget</t>
+  </si>
+  <si>
+    <t>Tune Senter</t>
+  </si>
+  <si>
+    <t>Adecco og If</t>
+  </si>
+  <si>
+    <t>Fagforbundet</t>
+  </si>
+  <si>
+    <t>Utenfor rundt Politiet</t>
   </si>
 </sst>
 </file>
@@ -449,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1183,4 +1208,136 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <f>SUM(B2:B13)</f>
+        <v>1370</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tidsinterval regning i Calc ark
</commit_message>
<xml_diff>
--- a/Resurser/kalkuleringsark.xlsx
+++ b/Resurser/kalkuleringsark.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henrik\Documents\GitHub\bach_current\Resurser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aga\Documents\GitHub\bach_current\Resurser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Inspiria</t>
   </si>
@@ -124,6 +124,24 @@
   </si>
   <si>
     <t>Fordelteprosenter</t>
+  </si>
+  <si>
+    <t>Tid/Ankomst</t>
+  </si>
+  <si>
+    <t>Tidsinterval</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>Biler</t>
+  </si>
+  <si>
+    <t>Totalt Biler</t>
+  </si>
+  <si>
+    <t>Interval/Biler</t>
   </si>
 </sst>
 </file>
@@ -167,13 +185,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -490,22 +515,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K43"/>
+  <dimension ref="B1:T43"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="N41" sqref="N41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -525,7 +552,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -548,7 +575,7 @@
         <v>0.18656716417910449</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -571,7 +598,7 @@
         <v>0.11194029850746269</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -594,7 +621,7 @@
         <v>0.11194029850746269</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -617,7 +644,7 @@
         <v>0.17164179104477612</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -640,7 +667,7 @@
         <v>0.16417910447761194</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -663,7 +690,7 @@
         <v>0.12686567164179105</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -686,7 +713,7 @@
         <v>4.4776119402985072E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -709,7 +736,7 @@
         <v>8.2089552238805971E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -734,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
@@ -742,7 +769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>520</v>
       </c>
@@ -756,7 +783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>545</v>
       </c>
@@ -776,7 +803,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>615</v>
       </c>
@@ -795,8 +822,15 @@
       <c r="K20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="3:20" ht="30" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>634</v>
       </c>
@@ -815,8 +849,27 @@
       <c r="K21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N21" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R21" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>645</v>
       </c>
@@ -835,8 +888,27 @@
       <c r="K22">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N22" s="7">
+        <v>700</v>
+      </c>
+      <c r="O22" s="7">
+        <v>0</v>
+      </c>
+      <c r="P22" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>0</v>
+      </c>
+      <c r="R22" s="7">
+        <v>0</v>
+      </c>
+      <c r="S22" s="7">
+        <v>0</v>
+      </c>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>655</v>
       </c>
@@ -855,8 +927,27 @@
       <c r="K23">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N23" s="7">
+        <v>705</v>
+      </c>
+      <c r="O23" s="7">
+        <v>30</v>
+      </c>
+      <c r="P23" s="7">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>77</v>
+      </c>
+      <c r="R23" s="7">
+        <v>77</v>
+      </c>
+      <c r="S23" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>705</v>
       </c>
@@ -875,8 +966,27 @@
       <c r="K24">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N24" s="7">
+        <v>715</v>
+      </c>
+      <c r="O24" s="7">
+        <v>60</v>
+      </c>
+      <c r="P24" s="7">
+        <v>90</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>48</v>
+      </c>
+      <c r="R24" s="7">
+        <v>125</v>
+      </c>
+      <c r="S24" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>715</v>
       </c>
@@ -895,8 +1005,27 @@
       <c r="K25">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N25" s="7">
+        <v>719</v>
+      </c>
+      <c r="O25" s="7">
+        <v>24</v>
+      </c>
+      <c r="P25" s="7">
+        <v>114</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>14</v>
+      </c>
+      <c r="R25" s="7">
+        <v>139</v>
+      </c>
+      <c r="S25" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>719</v>
       </c>
@@ -915,8 +1044,27 @@
       <c r="K26">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N26" s="7">
+        <v>730</v>
+      </c>
+      <c r="O26" s="7">
+        <v>66</v>
+      </c>
+      <c r="P26" s="7">
+        <v>180</v>
+      </c>
+      <c r="Q26" s="7">
+        <v>142</v>
+      </c>
+      <c r="R26" s="7">
+        <v>281</v>
+      </c>
+      <c r="S26" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T26" s="5"/>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>730</v>
       </c>
@@ -935,8 +1083,27 @@
       <c r="K27">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N27" s="7">
+        <v>739</v>
+      </c>
+      <c r="O27" s="7">
+        <v>54</v>
+      </c>
+      <c r="P27" s="7">
+        <v>234</v>
+      </c>
+      <c r="Q27" s="7">
+        <v>12</v>
+      </c>
+      <c r="R27" s="7">
+        <v>293</v>
+      </c>
+      <c r="S27" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="T27" s="5"/>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>739</v>
       </c>
@@ -955,8 +1122,27 @@
       <c r="K28">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N28" s="7">
+        <v>745</v>
+      </c>
+      <c r="O28" s="7">
+        <v>36</v>
+      </c>
+      <c r="P28" s="7">
+        <v>270</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>81</v>
+      </c>
+      <c r="R28" s="7">
+        <v>374</v>
+      </c>
+      <c r="S28" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T28" s="5"/>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>745</v>
       </c>
@@ -975,8 +1161,27 @@
       <c r="K29">
         <v>142</v>
       </c>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N29" s="7">
+        <v>752</v>
+      </c>
+      <c r="O29" s="7">
+        <v>42</v>
+      </c>
+      <c r="P29" s="7">
+        <v>312</v>
+      </c>
+      <c r="Q29" s="7">
+        <v>57</v>
+      </c>
+      <c r="R29" s="7">
+        <v>431</v>
+      </c>
+      <c r="S29" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="T29" s="5"/>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C30">
         <v>752</v>
       </c>
@@ -995,8 +1200,27 @@
       <c r="K30">
         <v>12</v>
       </c>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N30" s="7">
+        <v>756</v>
+      </c>
+      <c r="O30" s="7">
+        <v>24</v>
+      </c>
+      <c r="P30" s="7">
+        <v>336</v>
+      </c>
+      <c r="Q30" s="7">
+        <v>38</v>
+      </c>
+      <c r="R30" s="7">
+        <v>469</v>
+      </c>
+      <c r="S30" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="T30" s="5"/>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>756</v>
       </c>
@@ -1015,8 +1239,27 @@
       <c r="K31">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N31" s="7">
+        <v>805</v>
+      </c>
+      <c r="O31" s="7">
+        <v>54</v>
+      </c>
+      <c r="P31" s="7">
+        <v>390</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>372</v>
+      </c>
+      <c r="R31" s="7">
+        <v>841</v>
+      </c>
+      <c r="S31" s="7">
+        <v>6.9</v>
+      </c>
+      <c r="T31" s="5"/>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>805</v>
       </c>
@@ -1035,8 +1278,27 @@
       <c r="K32">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N32" s="7">
+        <v>815</v>
+      </c>
+      <c r="O32" s="7">
+        <v>60</v>
+      </c>
+      <c r="P32" s="7">
+        <v>450</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>42</v>
+      </c>
+      <c r="R32" s="7">
+        <v>883</v>
+      </c>
+      <c r="S32" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="T32" s="5"/>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C33">
         <v>815</v>
       </c>
@@ -1055,8 +1317,27 @@
       <c r="K33">
         <v>38</v>
       </c>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N33" s="7">
+        <v>830</v>
+      </c>
+      <c r="O33" s="7">
+        <v>90</v>
+      </c>
+      <c r="P33" s="7">
+        <v>540</v>
+      </c>
+      <c r="Q33" s="7">
+        <v>127</v>
+      </c>
+      <c r="R33" s="7">
+        <v>1010</v>
+      </c>
+      <c r="S33" s="7">
+        <v>1.4</v>
+      </c>
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C34">
         <v>830</v>
       </c>
@@ -1075,8 +1356,27 @@
       <c r="K34">
         <v>372</v>
       </c>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N34" s="7">
+        <v>845</v>
+      </c>
+      <c r="O34" s="7">
+        <v>90</v>
+      </c>
+      <c r="P34" s="7">
+        <v>630</v>
+      </c>
+      <c r="Q34" s="7">
+        <v>16</v>
+      </c>
+      <c r="R34" s="7">
+        <v>1026</v>
+      </c>
+      <c r="S34" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>845</v>
       </c>
@@ -1095,8 +1395,27 @@
       <c r="K35">
         <v>42</v>
       </c>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N35" s="7">
+        <v>911</v>
+      </c>
+      <c r="O35" s="7">
+        <v>156</v>
+      </c>
+      <c r="P35" s="7">
+        <v>786</v>
+      </c>
+      <c r="Q35" s="7">
+        <v>31</v>
+      </c>
+      <c r="R35" s="7">
+        <v>1057</v>
+      </c>
+      <c r="S35" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="T35" s="5"/>
+    </row>
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C36">
         <v>911</v>
       </c>
@@ -1115,8 +1434,27 @@
       <c r="K36">
         <v>127</v>
       </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N36" s="7">
+        <v>930</v>
+      </c>
+      <c r="O36" s="7">
+        <v>114</v>
+      </c>
+      <c r="P36" s="7">
+        <v>900</v>
+      </c>
+      <c r="Q36" s="7">
+        <v>12</v>
+      </c>
+      <c r="R36" s="7">
+        <v>1069</v>
+      </c>
+      <c r="S36" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="T36" s="5"/>
+    </row>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>930</v>
       </c>
@@ -1135,8 +1473,27 @@
       <c r="K37">
         <v>16</v>
       </c>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N37" s="7">
+        <v>1000</v>
+      </c>
+      <c r="O37" s="7">
+        <v>180</v>
+      </c>
+      <c r="P37" s="7">
+        <v>1080</v>
+      </c>
+      <c r="Q37" s="7">
+        <v>16</v>
+      </c>
+      <c r="R37" s="7">
+        <v>1085</v>
+      </c>
+      <c r="S37" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="T37" s="5"/>
+    </row>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>1000</v>
       </c>
@@ -1155,8 +1512,15 @@
       <c r="K38">
         <v>31</v>
       </c>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>1045</v>
       </c>
@@ -1176,8 +1540,15 @@
         <f>SUM(K20:K38)</f>
         <v>1112</v>
       </c>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="5"/>
+      <c r="T39" s="5"/>
+    </row>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>1300</v>
       </c>
@@ -1190,8 +1561,15 @@
       <c r="G40">
         <v>21</v>
       </c>
-    </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.3">
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+      <c r="P40" s="5"/>
+      <c r="Q40" s="5"/>
+      <c r="R40" s="5"/>
+      <c r="S40" s="5"/>
+      <c r="T40" s="5"/>
+    </row>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>11</v>
       </c>
@@ -1206,7 +1584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="F42">
         <v>2030</v>
       </c>
@@ -1214,7 +1592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
         <v>11</v>
       </c>
@@ -1225,6 +1603,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1232,21 +1611,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1269,7 +1648,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1296,7 +1675,7 @@
         <v>9.1240875912408759E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1323,7 +1702,7 @@
         <v>0.12043795620437955</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1350,7 +1729,7 @@
         <v>0.26642335766423353</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1377,7 +1756,7 @@
         <v>0.41605839416058388</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1404,7 +1783,7 @@
         <v>0.56934306569343063</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1431,7 +1810,7 @@
         <v>0.6934306569343065</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1458,7 +1837,7 @@
         <v>0.72627737226277367</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1485,7 +1864,7 @@
         <v>0.75547445255474444</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1512,7 +1891,7 @@
         <v>0.83941605839416045</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1539,7 +1918,7 @@
         <v>0.91970802919708017</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1566,7 +1945,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1591,7 +1970,7 @@
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1602,7 +1981,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1111</v>
       </c>

</xml_diff>